<commit_message>
modificados los sprites del dungeon
</commit_message>
<xml_diff>
--- a/Docs/Mapa.xlsx
+++ b/Docs/Mapa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Proyectos VS\Proyectazo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82E61C8-9F16-4C8D-9D2A-552569BC7ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B2C305-C06D-4BF1-A40C-91BD50D4F124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6030" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapa mejorado" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="21">
   <si>
     <t>d01</t>
   </si>
@@ -81,12 +81,15 @@
   <si>
     <t>s04</t>
   </si>
+  <si>
+    <t>w02</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +220,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1080,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH20" sqref="AH20"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:AZ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,19 +1428,19 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
@@ -1926,19 +1935,19 @@
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U6" t="s">
         <v>6</v>
@@ -2311,25 +2320,25 @@
         <v>4</v>
       </c>
       <c r="AM8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AN8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP8" t="s">
         <v>14</v>
       </c>
       <c r="AQ8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AS8" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AT8" t="s">
         <v>6</v>
@@ -2364,40 +2373,40 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P9" t="s">
         <v>5</v>
@@ -3154,22 +3163,22 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
@@ -3822,19 +3831,19 @@
         <v>4</v>
       </c>
       <c r="P18" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q18" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R18" t="s">
         <v>5</v>
       </c>
       <c r="S18" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T18" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U18" t="s">
         <v>6</v>
@@ -4615,7 +4624,7 @@
         <v>2</v>
       </c>
       <c r="Q23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R23" t="s">
         <v>5</v>
@@ -4764,25 +4773,25 @@
         <v>12</v>
       </c>
       <c r="N24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R24" t="s">
         <v>5</v>
       </c>
       <c r="S24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T24" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U24" t="s">
         <v>13</v>
@@ -4815,7 +4824,7 @@
         <v>2</v>
       </c>
       <c r="AE24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF24" t="s">
         <v>0</v>
@@ -4895,31 +4904,31 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N25" t="s">
         <v>5</v>
@@ -4943,34 +4952,34 @@
         <v>5</v>
       </c>
       <c r="U25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AB25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AC25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AD25" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AE25" t="s">
         <v>6</v>
@@ -5399,13 +5408,13 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P28" t="s">
         <v>5</v>
       </c>
       <c r="Q28" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R28" t="s">
         <v>0</v>
@@ -5447,7 +5456,7 @@
         <v>5</v>
       </c>
       <c r="AE28" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AF28" t="s">
         <v>2</v>
@@ -5474,19 +5483,19 @@
         <v>4</v>
       </c>
       <c r="AN28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP28" t="s">
         <v>5</v>
       </c>
       <c r="AQ28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AS28" t="s">
         <v>6</v>
@@ -5599,19 +5608,19 @@
         <v>4</v>
       </c>
       <c r="AC29" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AD29" t="s">
         <v>5</v>
       </c>
       <c r="AE29" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AF29" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AG29" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AH29" t="s">
         <v>6</v>
@@ -5715,16 +5724,16 @@
         <v>4</v>
       </c>
       <c r="O30" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P30" t="s">
         <v>5</v>
       </c>
       <c r="Q30" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R30" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S30" t="s">
         <v>13</v>
@@ -5885,25 +5894,25 @@
         <v>5</v>
       </c>
       <c r="S31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z31" t="s">
         <v>6</v>
@@ -6511,7 +6520,7 @@
         <v>5</v>
       </c>
       <c r="Q35" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R35" t="s">
         <v>0</v>
@@ -6669,7 +6678,7 @@
         <v>5</v>
       </c>
       <c r="Q36" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R36" t="s">
         <v>0</v>
@@ -6827,7 +6836,7 @@
         <v>5</v>
       </c>
       <c r="Q37" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R37" t="s">
         <v>0</v>
@@ -6985,7 +6994,7 @@
         <v>5</v>
       </c>
       <c r="Q38" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="R38" t="s">
         <v>2</v>
@@ -7063,25 +7072,25 @@
         <v>5</v>
       </c>
       <c r="AQ38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AS38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AT38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AU38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AV38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AW38" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AX38" t="s">
         <v>6</v>
@@ -7146,25 +7155,25 @@
         <v>5</v>
       </c>
       <c r="R39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X39" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y39" t="s">
         <v>5</v>
@@ -7736,31 +7745,31 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G43" t="s">
         <v>5</v>
       </c>
       <c r="H43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L43" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M43" t="s">
         <v>6</v>
@@ -7939,19 +7948,19 @@
         <v>12</v>
       </c>
       <c r="S44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W44" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X44" t="s">
         <v>13</v>
@@ -8079,22 +8088,22 @@
         <v>5</v>
       </c>
       <c r="M45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S45" t="s">
         <v>5</v>
@@ -8115,10 +8124,10 @@
         <v>19</v>
       </c>
       <c r="Y45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z45" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA45" t="s">
         <v>5</v>
@@ -8598,22 +8607,22 @@
         <v>5</v>
       </c>
       <c r="AB48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AC48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AD48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AE48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AF48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AG48" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AH48" t="s">
         <v>13</v>
@@ -8774,28 +8783,28 @@
         <v>5</v>
       </c>
       <c r="AH49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AI49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AJ49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AK49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AL49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AM49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AN49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO49" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP49" t="s">
         <v>6</v>
@@ -9176,55 +9185,55 @@
         <v>4</v>
       </c>
       <c r="J52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="M52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="N52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Q52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z52" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA52" t="s">
         <v>5</v>
@@ -9406,37 +9415,37 @@
         <v>5</v>
       </c>
       <c r="AH53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AI53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AJ53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AK53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AL53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AM53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AN53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AQ53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR53" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AS53" t="s">
         <v>6</v>
@@ -9829,34 +9838,34 @@
         <v>4</v>
       </c>
       <c r="Q56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="R56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z56" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA56" t="s">
         <v>5</v>
@@ -10047,16 +10056,16 @@
         <v>4</v>
       </c>
       <c r="AK57" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AL57" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AM57" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AN57" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO57" t="s">
         <v>13</v>
@@ -10217,13 +10226,13 @@
         <v>5</v>
       </c>
       <c r="AO58" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP58" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AQ58" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR58" t="s">
         <v>5</v>
@@ -10780,34 +10789,34 @@
         <v>5</v>
       </c>
       <c r="R62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="S62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="T62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="U62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="V62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Y62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="Z62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AA62" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AB62" t="s">
         <v>5</v>
@@ -10983,52 +10992,52 @@
         <v>5</v>
       </c>
       <c r="AG63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AH63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AI63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AJ63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AK63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AL63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AM63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AN63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AO63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AQ63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AR63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AS63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AT63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AU63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AV63" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AW63" t="s">
         <v>5</v>
@@ -11360,6 +11369,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A1:AZ1048576">
     <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
       <formula>"d01"</formula>

</xml_diff>